<commit_message>
Update blue colour, program demand constraint name finalized (saturation)
</commit_message>
<xml_diff>
--- a/tests/databooks/progbook_hiv.xlsx
+++ b/tests/databooks/progbook_hiv.xlsx
@@ -15,81 +15,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In this column, enter the baseline value for "Diagnosis rate" if none of the programs reach this parameter (e.g., if the coverage is 0)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In this column, enter the baseline value for "Average time taken to be linked to care (years)" if none of the programs reach this parameter (e.g., if the coverage is 0)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In this column, enter the baseline value for "Initiation rate" if none of the programs reach this parameter (e.g., if the coverage is 0)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In this column, enter the baseline value for "Loss-to-follow-up rate" if none of the programs reach this parameter (e.g., if the coverage is 0)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B17" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In this column, enter the baseline value for "Treatment failure rate" if none of the programs reach this parameter (e.g., if the coverage is 0)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="46">
   <si>
@@ -189,16 +114,16 @@
     <t>OR</t>
   </si>
   <si>
-    <t>Capacity constraints</t>
-  </si>
-  <si>
     <t>Unit cost</t>
   </si>
   <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Saturation</t>
+  </si>
+  <si>
     <t>Coverage</t>
-  </si>
-  <si>
-    <t>Demand constraint</t>
   </si>
   <si>
     <t>Diagnosis rate</t>
@@ -235,19 +160,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -267,7 +186,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF18C1FF"/>
+        <fgColor rgb="FF98E0FA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -320,22 +239,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -696,42 +613,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -742,28 +659,28 @@
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -774,28 +691,28 @@
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -806,28 +723,28 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -838,28 +755,28 @@
       <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -870,28 +787,28 @@
       <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -902,28 +819,28 @@
       <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -934,28 +851,28 @@
       <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1429,690 +1346,690 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2">
         <v>2015</v>
       </c>
-      <c r="F1" s="6">
+      <c r="F1" s="2">
         <v>2016</v>
       </c>
-      <c r="G1" s="6">
+      <c r="G1" s="2">
         <v>2017</v>
       </c>
-      <c r="H1" s="6">
+      <c r="H1" s="2">
         <v>2018</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6">
         <v>15000000</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6">
+        <v>100</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>2015</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2017</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6">
+        <v>6000000</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6">
         <v>100</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="3" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="5" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="3" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="5" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2">
         <v>2015</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F15" s="2">
         <v>2016</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G15" s="2">
         <v>2017</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H15" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3" t="s">
+    <row r="16" spans="1:8">
+      <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="5" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8">
-        <v>6000000</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="3" t="s">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6">
+        <v>60000000</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="3" t="s">
+      <c r="E17" s="6"/>
+      <c r="F17" s="6">
+        <v>200</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="5" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8">
-        <v>100</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="3" t="s">
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="3" t="s">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2">
         <v>2015</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F22" s="2">
         <v>2016</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G22" s="2">
         <v>2017</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H22" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="3" t="s">
+    <row r="23" spans="1:8">
+      <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="5" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8">
-        <v>60000000</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="3" t="s">
+      <c r="E23" s="6"/>
+      <c r="F23" s="6">
+        <v>45000000</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="5" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="3" t="s">
+      <c r="E24" s="6"/>
+      <c r="F24" s="6">
+        <v>300</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="5" t="s">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8">
-        <v>200</v>
-      </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="3" t="s">
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5" t="s">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="3" t="s">
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="5" t="s">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="6" t="s">
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2">
         <v>2015</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F29" s="2">
         <v>2016</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G29" s="2">
         <v>2017</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H29" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="3" t="s">
+    <row r="30" spans="1:8">
+      <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="5" t="s">
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8">
-        <v>45000000</v>
-      </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="3" t="s">
+      <c r="E30" s="6"/>
+      <c r="F30" s="6">
+        <v>600000</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="3" t="s">
+      <c r="E31" s="6"/>
+      <c r="F31" s="6">
+        <v>60</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="5" t="s">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8">
-        <v>300</v>
-      </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="3" t="s">
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="5" t="s">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="3" t="s">
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="5" t="s">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="6" t="s">
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C36" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2">
         <v>2015</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F36" s="2">
         <v>2016</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G36" s="2">
         <v>2017</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H36" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="3" t="s">
+    <row r="37" spans="1:8">
+      <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="5" t="s">
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8">
+      <c r="E37" s="6"/>
+      <c r="F37" s="6">
         <v>600000</v>
       </c>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="3" t="s">
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="5" t="s">
+      <c r="B38" s="5"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="3" t="s">
+      <c r="E38" s="6"/>
+      <c r="F38" s="6">
+        <v>150</v>
+      </c>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="5" t="s">
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8">
-        <v>60</v>
-      </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="3" t="s">
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="5" t="s">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="3" t="s">
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="5" t="s">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="6" t="s">
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C43" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6">
+      <c r="D43" s="2"/>
+      <c r="E43" s="2">
         <v>2015</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F43" s="2">
         <v>2016</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G43" s="2">
         <v>2017</v>
       </c>
-      <c r="H36" s="6">
+      <c r="H43" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="3" t="s">
+    <row r="44" spans="1:8">
+      <c r="A44" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="5" t="s">
+      <c r="B44" s="5"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8">
-        <v>600000</v>
-      </c>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="3" t="s">
+      <c r="E44" s="6"/>
+      <c r="F44" s="6">
+        <v>10000</v>
+      </c>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="5" t="s">
+      <c r="B45" s="5"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="3" t="s">
+      <c r="E45" s="6"/>
+      <c r="F45" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="5" t="s">
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8">
-        <v>150</v>
-      </c>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="3" t="s">
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="5" t="s">
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="3" t="s">
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="5" t="s">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6">
-        <v>2015</v>
-      </c>
-      <c r="F43" s="6">
-        <v>2016</v>
-      </c>
-      <c r="G43" s="6">
-        <v>2017</v>
-      </c>
-      <c r="H43" s="6">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8">
-        <v>10000</v>
-      </c>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C10">
@@ -2422,46 +2339,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="3" t="str">
+      <c r="G1" s="2" t="str">
         <f>'Program targeting'!$A$3</f>
         <v>Testing - clinics</v>
       </c>
-      <c r="H1" s="3" t="str">
+      <c r="H1" s="2" t="str">
         <f>'Program targeting'!$A$4</f>
         <v>Testing - outreach</v>
       </c>
-      <c r="I1" s="3" t="str">
+      <c r="I1" s="2" t="str">
         <f>'Program targeting'!$A$5</f>
         <v>Same-day initiation counselling</v>
       </c>
-      <c r="J1" s="3" t="str">
+      <c r="J1" s="2" t="str">
         <f>'Program targeting'!$A$6</f>
         <v>Classic initiation counselling</v>
       </c>
-      <c r="K1" s="3" t="str">
+      <c r="K1" s="2" t="str">
         <f>'Program targeting'!$A$7</f>
         <v>Client tracing</v>
       </c>
-      <c r="L1" s="3" t="str">
+      <c r="L1" s="2" t="str">
         <f>'Program targeting'!$A$8</f>
         <v>Advanced adherence support</v>
       </c>
-      <c r="M1" s="3" t="str">
+      <c r="M1" s="2" t="str">
         <f>'Program targeting'!$A$9</f>
         <v>Whatsapp adherence support</v>
       </c>
@@ -2471,92 +2388,92 @@
         <f>'Program targeting'!$C$2</f>
         <v>Females</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="G2" s="8">
+      <c r="E2" s="5"/>
+      <c r="G2" s="6">
         <v>1</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="6">
         <v>1</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="str">
         <f>'Program targeting'!$D$2</f>
         <v>Males</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
+      <c r="E3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="3" t="str">
+      <c r="G5" s="2" t="str">
         <f>'Program targeting'!$A$3</f>
         <v>Testing - clinics</v>
       </c>
-      <c r="H5" s="3" t="str">
+      <c r="H5" s="2" t="str">
         <f>'Program targeting'!$A$4</f>
         <v>Testing - outreach</v>
       </c>
-      <c r="I5" s="3" t="str">
+      <c r="I5" s="2" t="str">
         <f>'Program targeting'!$A$5</f>
         <v>Same-day initiation counselling</v>
       </c>
-      <c r="J5" s="3" t="str">
+      <c r="J5" s="2" t="str">
         <f>'Program targeting'!$A$6</f>
         <v>Classic initiation counselling</v>
       </c>
-      <c r="K5" s="3" t="str">
+      <c r="K5" s="2" t="str">
         <f>'Program targeting'!$A$7</f>
         <v>Client tracing</v>
       </c>
-      <c r="L5" s="3" t="str">
+      <c r="L5" s="2" t="str">
         <f>'Program targeting'!$A$8</f>
         <v>Advanced adherence support</v>
       </c>
-      <c r="M5" s="3" t="str">
+      <c r="M5" s="2" t="str">
         <f>'Program targeting'!$A$9</f>
         <v>Whatsapp adherence support</v>
       </c>
@@ -2566,100 +2483,100 @@
         <f>'Program targeting'!$C$2</f>
         <v>Females</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>1.5</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="G6" s="8">
+      <c r="E6" s="5"/>
+      <c r="G6" s="6">
         <v>0.5</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="6">
         <v>0.3</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="8">
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="6">
         <v>0.2</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="str">
         <f>'Program targeting'!$D$2</f>
         <v>Males</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>2.2</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="G7" s="8">
+      <c r="E7" s="5"/>
+      <c r="G7" s="6">
         <v>0.6</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="6">
         <v>0.4</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="8">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="6">
         <v>0.3</v>
       </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="3" t="str">
+      <c r="G9" s="2" t="str">
         <f>'Program targeting'!$A$3</f>
         <v>Testing - clinics</v>
       </c>
-      <c r="H9" s="3" t="str">
+      <c r="H9" s="2" t="str">
         <f>'Program targeting'!$A$4</f>
         <v>Testing - outreach</v>
       </c>
-      <c r="I9" s="3" t="str">
+      <c r="I9" s="2" t="str">
         <f>'Program targeting'!$A$5</f>
         <v>Same-day initiation counselling</v>
       </c>
-      <c r="J9" s="3" t="str">
+      <c r="J9" s="2" t="str">
         <f>'Program targeting'!$A$6</f>
         <v>Classic initiation counselling</v>
       </c>
-      <c r="K9" s="3" t="str">
+      <c r="K9" s="2" t="str">
         <f>'Program targeting'!$A$7</f>
         <v>Client tracing</v>
       </c>
-      <c r="L9" s="3" t="str">
+      <c r="L9" s="2" t="str">
         <f>'Program targeting'!$A$8</f>
         <v>Advanced adherence support</v>
       </c>
-      <c r="M9" s="3" t="str">
+      <c r="M9" s="2" t="str">
         <f>'Program targeting'!$A$9</f>
         <v>Whatsapp adherence support</v>
       </c>
@@ -2669,92 +2586,92 @@
         <f>'Program targeting'!$C$2</f>
         <v>Females</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>0</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="8">
+      <c r="E10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6">
         <v>0.98</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="6">
         <v>0.92</v>
       </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="str">
         <f>'Program targeting'!$D$2</f>
         <v>Males</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>0</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="E11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="3" t="str">
+      <c r="G13" s="2" t="str">
         <f>'Program targeting'!$A$3</f>
         <v>Testing - clinics</v>
       </c>
-      <c r="H13" s="3" t="str">
+      <c r="H13" s="2" t="str">
         <f>'Program targeting'!$A$4</f>
         <v>Testing - outreach</v>
       </c>
-      <c r="I13" s="3" t="str">
+      <c r="I13" s="2" t="str">
         <f>'Program targeting'!$A$5</f>
         <v>Same-day initiation counselling</v>
       </c>
-      <c r="J13" s="3" t="str">
+      <c r="J13" s="2" t="str">
         <f>'Program targeting'!$A$6</f>
         <v>Classic initiation counselling</v>
       </c>
-      <c r="K13" s="3" t="str">
+      <c r="K13" s="2" t="str">
         <f>'Program targeting'!$A$7</f>
         <v>Client tracing</v>
       </c>
-      <c r="L13" s="3" t="str">
+      <c r="L13" s="2" t="str">
         <f>'Program targeting'!$A$8</f>
         <v>Advanced adherence support</v>
       </c>
-      <c r="M13" s="3" t="str">
+      <c r="M13" s="2" t="str">
         <f>'Program targeting'!$A$9</f>
         <v>Whatsapp adherence support</v>
       </c>
@@ -2764,25 +2681,25 @@
         <f>'Program targeting'!$C$2</f>
         <v>Females</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="6">
         <v>0.5</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="8">
+      <c r="E14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="6">
         <v>0.1</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M14" s="6">
         <v>0.2</v>
       </c>
     </row>
@@ -2791,69 +2708,69 @@
         <f>'Program targeting'!$D$2</f>
         <v>Males</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="6">
         <v>0.7</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="8">
+      <c r="E15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="6">
         <v>0.15</v>
       </c>
-      <c r="M15" s="8">
+      <c r="M15" s="6">
         <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="3" t="str">
+      <c r="G17" s="2" t="str">
         <f>'Program targeting'!$A$3</f>
         <v>Testing - clinics</v>
       </c>
-      <c r="H17" s="3" t="str">
+      <c r="H17" s="2" t="str">
         <f>'Program targeting'!$A$4</f>
         <v>Testing - outreach</v>
       </c>
-      <c r="I17" s="3" t="str">
+      <c r="I17" s="2" t="str">
         <f>'Program targeting'!$A$5</f>
         <v>Same-day initiation counselling</v>
       </c>
-      <c r="J17" s="3" t="str">
+      <c r="J17" s="2" t="str">
         <f>'Program targeting'!$A$6</f>
         <v>Classic initiation counselling</v>
       </c>
-      <c r="K17" s="3" t="str">
+      <c r="K17" s="2" t="str">
         <f>'Program targeting'!$A$7</f>
         <v>Client tracing</v>
       </c>
-      <c r="L17" s="3" t="str">
+      <c r="L17" s="2" t="str">
         <f>'Program targeting'!$A$8</f>
         <v>Advanced adherence support</v>
       </c>
-      <c r="M17" s="3" t="str">
+      <c r="M17" s="2" t="str">
         <f>'Program targeting'!$A$9</f>
         <v>Whatsapp adherence support</v>
       </c>
@@ -2863,25 +2780,25 @@
         <f>'Program targeting'!$C$2</f>
         <v>Females</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>0.3</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="8">
+      <c r="E18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="6">
         <v>0.1</v>
       </c>
-      <c r="M18" s="8">
+      <c r="M18" s="6">
         <v>0.15</v>
       </c>
     </row>
@@ -2890,25 +2807,25 @@
         <f>'Program targeting'!$D$2</f>
         <v>Males</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="6">
         <v>0.4</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="8">
+      <c r="E19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="6">
         <v>0.15</v>
       </c>
-      <c r="M19" s="8">
+      <c r="M19" s="6">
         <v>0.2</v>
       </c>
     </row>
@@ -3536,6 +3453,5 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>